<commit_message>
lsl-- add cms core  DataAccess
add cms core  DataAccess
</commit_message>
<xml_diff>
--- a/CMS/CMS_TIP/TA_BASE/transactive/test/TestCase/TestCaseCMSServer/doc/CMS_TCP_Test.xlsx
+++ b/CMS/CMS_TIP/TA_BASE/transactive/test/TestCase/TestCaseCMSServer/doc/CMS_TCP_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="110">
   <si>
     <t>测试环境</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -250,149 +250,171 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>发送各种类型的最小值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送各种类型的最大值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>断开连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重复读取数据帧的内容(Message)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（不打log)</t>
+  </si>
+  <si>
+    <t>10个客户端</t>
+  </si>
+  <si>
+    <t>一共 10*100000</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>32位</t>
+  </si>
+  <si>
+    <t xml:space="preserve">windows7 </t>
+  </si>
+  <si>
+    <t>局域网</t>
+  </si>
+  <si>
+    <t>网络正常</t>
+  </si>
+  <si>
+    <t>基本功能</t>
+  </si>
+  <si>
+    <t>服务端数量1</t>
+  </si>
+  <si>
+    <t>发送各种类型的正常值（100000个帧）</t>
+  </si>
+  <si>
+    <t>100个客户端</t>
+  </si>
+  <si>
+    <t>一共100*100000</t>
+  </si>
+  <si>
+    <t>（客户端 服务端分别为一个进程）</t>
+  </si>
+  <si>
+    <t>1个客户端</t>
+  </si>
+  <si>
+    <t>接收使用时间： 135206 ms</t>
+  </si>
+  <si>
+    <t>（服务端为一个进程, 客户端 为100个进程）</t>
+  </si>
+  <si>
+    <t>发送使用时间： 22797 ms</t>
+  </si>
+  <si>
+    <t>接收使用时间：9696 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1355 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：260 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1351 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1399 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：2710 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：2721 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1345 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1940 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：2857 ms</t>
+  </si>
+  <si>
+    <t>（服务端分别为一个进程， 客户端为10个进程）</t>
+  </si>
+  <si>
+    <t>发送使用时间：381 ms</t>
+  </si>
+  <si>
+    <t>接收使用时间：989 ms</t>
+  </si>
+  <si>
+    <t>服务端不再收到数据，handleDisconnected 和 handleDeliverFailure 一直再被回调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送过程中客户端异常断开连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送过程中服务端异常断开连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户端不再收到数据，handleDisconnected 被回调一次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>472个客户端</t>
+  </si>
+  <si>
     <t>发送各种类型的正常值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送各种类型的最小值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送各种类型的最大值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>断开连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>读取数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sting&lt;256, void* 没有测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重复读取数据帧的内容(Message)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>（不打log)</t>
-  </si>
-  <si>
-    <t>10个客户端</t>
-  </si>
-  <si>
-    <t>一共 10*100000</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>32位</t>
-  </si>
-  <si>
-    <t xml:space="preserve">windows7 </t>
-  </si>
-  <si>
-    <t>局域网</t>
-  </si>
-  <si>
-    <t>网络正常</t>
-  </si>
-  <si>
-    <t>基本功能</t>
-  </si>
-  <si>
-    <t>服务端数量1</t>
-  </si>
-  <si>
-    <t>发送各种类型的正常值（100000个帧）</t>
-  </si>
-  <si>
-    <t>100个客户端</t>
-  </si>
-  <si>
-    <t>一共100*100000</t>
-  </si>
-  <si>
-    <t>（客户端 服务端分别为一个进程）</t>
-  </si>
-  <si>
-    <t>1个客户端</t>
-  </si>
-  <si>
-    <t>接收使用时间： 135206 ms</t>
-  </si>
-  <si>
-    <t>（服务端为一个进程, 客户端 为100个进程）</t>
-  </si>
-  <si>
-    <t>发送使用时间： 22797 ms</t>
-  </si>
-  <si>
-    <t>接收使用时间：9696 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1355 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：260 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1351 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1399 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：2710 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：2721 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1345 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1940 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：2857 ms</t>
-  </si>
-  <si>
-    <t>（服务端分别为一个进程， 客户端为10个进程）</t>
-  </si>
-  <si>
-    <t>发送使用时间：381 ms</t>
-  </si>
-  <si>
-    <t>接收使用时间：989 ms</t>
-  </si>
-  <si>
-    <t>服务端不再收到数据，handleDisconnected 和 handleDeliverFailure 一直再被回调</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送过程中客户端异常断开连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送过程中服务端异常断开连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>客户端不再收到数据，handleDisconnected 被回调一次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string&lt;256, void* 没有测试</t>
+  </si>
+  <si>
+    <t>一个客户端进程，创建500个客户端线程，connecte 500, handleConnected 只被回调472次</t>
+  </si>
+  <si>
+    <t>数据发送正常，运行一天</t>
+  </si>
+  <si>
+    <t>490个客户端</t>
+  </si>
+  <si>
+    <t>250个客户端</t>
+  </si>
+  <si>
+    <t>一个客户端进程，创建490个客户端线程，connecte 490, handleConnected 被回调490次</t>
+  </si>
+  <si>
+    <t>数据发送正常，监控中</t>
+  </si>
+  <si>
+    <t>一个客户端进程，创建250个客户端线程，connecte 250, handleConnected 被回调250次</t>
   </si>
 </sst>
 </file>
@@ -403,13 +425,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -418,7 +440,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -426,21 +448,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -812,23 +834,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="6" width="17" style="2"/>
-    <col min="7" max="7" width="22.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="17" style="2"/>
-    <col min="9" max="9" width="22.875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="25.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" style="2" customWidth="1"/>
     <col min="12" max="16384" width="17" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40.5">
+    <row r="1" spans="1:11" ht="75">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="30">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,7 +885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -898,7 +920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,7 +955,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="30">
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
@@ -995,25 +1017,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="9.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="7" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="11" width="30.875" customWidth="1"/>
-    <col min="12" max="12" width="35.25" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="13.875" customWidth="1"/>
-    <col min="15" max="15" width="43.875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" customWidth="1"/>
+    <col min="11" max="11" width="88.140625" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1055,7 +1077,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
@@ -1079,7 +1101,7 @@
         <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1108,7 +1130,7 @@
         <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1137,12 +1159,12 @@
         <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
@@ -1166,7 +1188,7 @@
         <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1195,7 +1217,7 @@
         <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1224,7 +1246,7 @@
         <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1253,92 +1275,92 @@
         <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1">
       <c r="B11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="K11" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="3" customFormat="1">
       <c r="B13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="K13" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1">
@@ -1346,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="3" customFormat="1">
@@ -1354,7 +1376,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1">
@@ -1362,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:15" s="3" customFormat="1">
@@ -1370,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:15" s="3" customFormat="1">
@@ -1378,7 +1400,7 @@
         <v>6</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:15" s="3" customFormat="1">
@@ -1386,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:15" s="3" customFormat="1">
@@ -1394,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:15" s="3" customFormat="1">
@@ -1402,7 +1424,7 @@
         <v>9</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="2:15" s="3" customFormat="1">
@@ -1410,63 +1432,63 @@
         <v>10</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:15" s="5" customFormat="1">
       <c r="B25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="G25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="K25" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:15" s="5" customFormat="1">
       <c r="J26" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="2:15" s="5" customFormat="1"/>
     <row r="28" spans="2:15" s="5" customFormat="1"/>
     <row r="30" spans="2:15">
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
@@ -1490,10 +1512,10 @@
         <v>55</v>
       </c>
       <c r="J30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="2:15">
@@ -1522,10 +1544,150 @@
         <v>55</v>
       </c>
       <c r="J31" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" t="s">
         <v>100</v>
       </c>
-      <c r="K31" t="s">
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" t="s">
         <v>101</v>
+      </c>
+      <c r="K33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" t="s">
+        <v>107</v>
+      </c>
+      <c r="L34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J36" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L37" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1540,7 +1702,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lsl -- add CFD sserver
lsl -- add CFD sserver
</commit_message>
<xml_diff>
--- a/CMS/CMS_TIP/TA_BASE/transactive/test/TestCase/TestCaseCMSServer/doc/CMS_TCP_Test.xlsx
+++ b/CMS/CMS_TIP/TA_BASE/transactive/test/TestCase/TestCaseCMSServer/doc/CMS_TCP_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
   <si>
     <t>测试环境</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -250,6 +250,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>发送各种类型的正常值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>发送各种类型的最小值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -274,6 +278,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>sting&lt;256, void* 没有测试</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>重复读取数据帧的内容(Message)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -385,36 +393,6 @@
   <si>
     <t>客户端不再收到数据，handleDisconnected 被回调一次</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>472个客户端</t>
-  </si>
-  <si>
-    <t>发送各种类型的正常值</t>
-  </si>
-  <si>
-    <t>string&lt;256, void* 没有测试</t>
-  </si>
-  <si>
-    <t>一个客户端进程，创建500个客户端线程，connecte 500, handleConnected 只被回调472次</t>
-  </si>
-  <si>
-    <t>数据发送正常，运行一天</t>
-  </si>
-  <si>
-    <t>490个客户端</t>
-  </si>
-  <si>
-    <t>250个客户端</t>
-  </si>
-  <si>
-    <t>一个客户端进程，创建490个客户端线程，connecte 490, handleConnected 被回调490次</t>
-  </si>
-  <si>
-    <t>数据发送正常，监控中</t>
-  </si>
-  <si>
-    <t>一个客户端进程，创建250个客户端线程，connecte 250, handleConnected 被回调250次</t>
   </si>
 </sst>
 </file>
@@ -425,13 +403,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -440,7 +418,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -448,21 +426,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -834,23 +812,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="6" width="17" style="2"/>
-    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.375" style="2" customWidth="1"/>
     <col min="8" max="8" width="17" style="2"/>
-    <col min="9" max="9" width="22.85546875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="25.85546875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="29.375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.875" style="2" customWidth="1"/>
     <col min="12" max="16384" width="17" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="75">
+    <row r="1" spans="1:11" ht="40.5">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1" ht="30">
+    <row r="3" spans="1:11" s="1" customFormat="1">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -885,7 +863,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="30">
+    <row r="4" spans="1:11">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -920,7 +898,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="30">
+    <row r="5" spans="1:11">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -955,7 +933,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="30">
+    <row r="6" spans="1:11">
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1017,25 +995,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O37"/>
+  <dimension ref="A1:O31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
-    <col min="5" max="5" width="9.5703125" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="14.140625" customWidth="1"/>
+    <col min="5" max="5" width="9.625" customWidth="1"/>
+    <col min="6" max="6" width="12.125" customWidth="1"/>
+    <col min="7" max="7" width="14.125" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="14.42578125" customWidth="1"/>
-    <col min="10" max="10" width="38.42578125" customWidth="1"/>
-    <col min="11" max="11" width="88.140625" customWidth="1"/>
-    <col min="12" max="12" width="35.28515625" customWidth="1"/>
-    <col min="13" max="13" width="14.7109375" customWidth="1"/>
-    <col min="14" max="14" width="13.85546875" customWidth="1"/>
-    <col min="15" max="15" width="43.85546875" customWidth="1"/>
+    <col min="9" max="9" width="14.375" customWidth="1"/>
+    <col min="10" max="10" width="38.375" customWidth="1"/>
+    <col min="11" max="11" width="30.875" customWidth="1"/>
+    <col min="12" max="12" width="35.25" customWidth="1"/>
+    <col min="13" max="13" width="14.75" customWidth="1"/>
+    <col min="14" max="14" width="13.875" customWidth="1"/>
+    <col min="15" max="15" width="43.875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1077,7 +1055,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
@@ -1101,7 +1079,7 @@
         <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1130,7 +1108,7 @@
         <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1159,12 +1137,12 @@
         <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
@@ -1188,7 +1166,7 @@
         <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1217,7 +1195,7 @@
         <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>101</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1246,7 +1224,7 @@
         <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1275,92 +1253,92 @@
         <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="K9" t="s">
-        <v>102</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1">
       <c r="B11" s="4" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="3" customFormat="1">
       <c r="B13" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="G13" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D13" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="F13" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>66</v>
-      </c>
       <c r="H13" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="J13" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1">
@@ -1368,7 +1346,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="3" customFormat="1">
@@ -1376,7 +1354,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1">
@@ -1384,7 +1362,7 @@
         <v>4</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="2:15" s="3" customFormat="1">
@@ -1392,7 +1370,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="18" spans="2:15" s="3" customFormat="1">
@@ -1400,7 +1378,7 @@
         <v>6</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="19" spans="2:15" s="3" customFormat="1">
@@ -1408,7 +1386,7 @@
         <v>7</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="2:15" s="3" customFormat="1">
@@ -1416,7 +1394,7 @@
         <v>8</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="21" spans="2:15" s="3" customFormat="1">
@@ -1424,7 +1402,7 @@
         <v>9</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="2:15" s="3" customFormat="1">
@@ -1432,63 +1410,63 @@
         <v>10</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="2:15" s="5" customFormat="1">
       <c r="B25" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="G25" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H25" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I25" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="H25" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="I25" s="5" t="s">
-        <v>74</v>
-      </c>
       <c r="J25" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="K25" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="L25" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="L25" s="5" t="s">
-        <v>80</v>
-      </c>
       <c r="M25" s="5" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="26" spans="2:15" s="5" customFormat="1">
       <c r="J26" s="5" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="27" spans="2:15" s="5" customFormat="1"/>
     <row r="28" spans="2:15" s="5" customFormat="1"/>
     <row r="30" spans="2:15">
       <c r="B30" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
@@ -1512,10 +1490,10 @@
         <v>55</v>
       </c>
       <c r="J30" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="K30" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="2:15">
@@ -1544,150 +1522,10 @@
         <v>55</v>
       </c>
       <c r="J31" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K31" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="33" spans="2:12">
-      <c r="B33" t="s">
-        <v>60</v>
-      </c>
-      <c r="C33" t="s">
-        <v>1</v>
-      </c>
-      <c r="D33" t="s">
-        <v>49</v>
-      </c>
-      <c r="E33" t="s">
-        <v>6</v>
-      </c>
-      <c r="F33" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" t="s">
-        <v>100</v>
-      </c>
-      <c r="H33" t="s">
-        <v>18</v>
-      </c>
-      <c r="I33" t="s">
-        <v>26</v>
-      </c>
-      <c r="J33" t="s">
         <v>101</v>
-      </c>
-      <c r="K33" t="s">
-        <v>103</v>
-      </c>
-      <c r="L33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="2:12">
-      <c r="B34" t="s">
-        <v>68</v>
-      </c>
-      <c r="C34" t="s">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" t="s">
-        <v>15</v>
-      </c>
-      <c r="G34" t="s">
-        <v>105</v>
-      </c>
-      <c r="H34" t="s">
-        <v>18</v>
-      </c>
-      <c r="I34" t="s">
-        <v>26</v>
-      </c>
-      <c r="J34" t="s">
-        <v>101</v>
-      </c>
-      <c r="K34" t="s">
-        <v>107</v>
-      </c>
-      <c r="L34" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12">
-      <c r="B36" t="s">
-        <v>68</v>
-      </c>
-      <c r="C36" t="s">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" t="s">
-        <v>106</v>
-      </c>
-      <c r="H36" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" t="s">
-        <v>26</v>
-      </c>
-      <c r="J36" t="s">
-        <v>101</v>
-      </c>
-      <c r="K36" t="s">
-        <v>109</v>
-      </c>
-      <c r="L36" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="37" spans="2:12">
-      <c r="B37" t="s">
-        <v>68</v>
-      </c>
-      <c r="C37" t="s">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
-        <v>49</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" t="s">
-        <v>106</v>
-      </c>
-      <c r="H37" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" t="s">
-        <v>26</v>
-      </c>
-      <c r="J37" t="s">
-        <v>101</v>
-      </c>
-      <c r="K37" t="s">
-        <v>109</v>
-      </c>
-      <c r="L37" t="s">
-        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1702,7 +1540,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
lsl -- add cfd server process Market data
-- add cfd server process Market data
</commit_message>
<xml_diff>
--- a/CMS/CMS_TIP/TA_BASE/transactive/test/TestCase/TestCaseCMSServer/doc/CMS_TCP_Test.xlsx
+++ b/CMS/CMS_TIP/TA_BASE/transactive/test/TestCase/TestCaseCMSServer/doc/CMS_TCP_Test.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="192" uniqueCount="102">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="110">
   <si>
     <t>测试环境</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -250,149 +250,171 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>发送各种类型的最小值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送各种类型的最大值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Error</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>断开连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>重复读取数据帧的内容(Message)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>（不打log)</t>
+  </si>
+  <si>
+    <t>10个客户端</t>
+  </si>
+  <si>
+    <t>一共 10*100000</t>
+  </si>
+  <si>
+    <t>OK</t>
+  </si>
+  <si>
+    <t>32位</t>
+  </si>
+  <si>
+    <t xml:space="preserve">windows7 </t>
+  </si>
+  <si>
+    <t>局域网</t>
+  </si>
+  <si>
+    <t>网络正常</t>
+  </si>
+  <si>
+    <t>基本功能</t>
+  </si>
+  <si>
+    <t>服务端数量1</t>
+  </si>
+  <si>
+    <t>发送各种类型的正常值（100000个帧）</t>
+  </si>
+  <si>
+    <t>100个客户端</t>
+  </si>
+  <si>
+    <t>一共100*100000</t>
+  </si>
+  <si>
+    <t>（客户端 服务端分别为一个进程）</t>
+  </si>
+  <si>
+    <t>1个客户端</t>
+  </si>
+  <si>
+    <t>接收使用时间： 135206 ms</t>
+  </si>
+  <si>
+    <t>（服务端为一个进程, 客户端 为100个进程）</t>
+  </si>
+  <si>
+    <t>发送使用时间： 22797 ms</t>
+  </si>
+  <si>
+    <t>接收使用时间：9696 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1355 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：260 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1351 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1399 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：2710 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：2721 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1345 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：1940 ms</t>
+  </si>
+  <si>
+    <t>发送使用时间：2857 ms</t>
+  </si>
+  <si>
+    <t>（服务端分别为一个进程， 客户端为10个进程）</t>
+  </si>
+  <si>
+    <t>发送使用时间：381 ms</t>
+  </si>
+  <si>
+    <t>接收使用时间：989 ms</t>
+  </si>
+  <si>
+    <t>服务端不再收到数据，handleDisconnected 和 handleDeliverFailure 一直再被回调</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送过程中客户端异常断开连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>发送过程中服务端异常断开连接</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>客户端不再收到数据，handleDisconnected 被回调一次</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>472个客户端</t>
+  </si>
+  <si>
     <t>发送各种类型的正常值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送各种类型的最小值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送各种类型的最大值</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Error</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>断开连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>读取数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>sting&lt;256, void* 没有测试</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>重复读取数据帧的内容(Message)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>（不打log)</t>
-  </si>
-  <si>
-    <t>10个客户端</t>
-  </si>
-  <si>
-    <t>一共 10*100000</t>
-  </si>
-  <si>
-    <t>OK</t>
-  </si>
-  <si>
-    <t>32位</t>
-  </si>
-  <si>
-    <t xml:space="preserve">windows7 </t>
-  </si>
-  <si>
-    <t>局域网</t>
-  </si>
-  <si>
-    <t>网络正常</t>
-  </si>
-  <si>
-    <t>基本功能</t>
-  </si>
-  <si>
-    <t>服务端数量1</t>
-  </si>
-  <si>
-    <t>发送各种类型的正常值（100000个帧）</t>
-  </si>
-  <si>
-    <t>100个客户端</t>
-  </si>
-  <si>
-    <t>一共100*100000</t>
-  </si>
-  <si>
-    <t>（客户端 服务端分别为一个进程）</t>
-  </si>
-  <si>
-    <t>1个客户端</t>
-  </si>
-  <si>
-    <t>接收使用时间： 135206 ms</t>
-  </si>
-  <si>
-    <t>（服务端为一个进程, 客户端 为100个进程）</t>
-  </si>
-  <si>
-    <t>发送使用时间： 22797 ms</t>
-  </si>
-  <si>
-    <t>接收使用时间：9696 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1355 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：260 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1351 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1399 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：2710 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：2721 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1345 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：1940 ms</t>
-  </si>
-  <si>
-    <t>发送使用时间：2857 ms</t>
-  </si>
-  <si>
-    <t>（服务端分别为一个进程， 客户端为10个进程）</t>
-  </si>
-  <si>
-    <t>发送使用时间：381 ms</t>
-  </si>
-  <si>
-    <t>接收使用时间：989 ms</t>
-  </si>
-  <si>
-    <t>服务端不再收到数据，handleDisconnected 和 handleDeliverFailure 一直再被回调</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送过程中客户端异常断开连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>发送过程中服务端异常断开连接</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>客户端不再收到数据，handleDisconnected 被回调一次</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>string&lt;256, void* 没有测试</t>
+  </si>
+  <si>
+    <t>一个客户端进程，创建500个客户端线程，connecte 500, handleConnected 只被回调472次</t>
+  </si>
+  <si>
+    <t>数据发送正常，运行一天</t>
+  </si>
+  <si>
+    <t>490个客户端</t>
+  </si>
+  <si>
+    <t>250个客户端</t>
+  </si>
+  <si>
+    <t>一个客户端进程，创建490个客户端线程，connecte 490, handleConnected 被回调490次</t>
+  </si>
+  <si>
+    <t>数据发送正常，监控中</t>
+  </si>
+  <si>
+    <t>一个客户端进程，创建250个客户端线程，connecte 250, handleConnected 被回调250次</t>
   </si>
 </sst>
 </file>
@@ -403,13 +425,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="9"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -418,7 +440,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -426,21 +448,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FF006100"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="宋体"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -812,23 +834,23 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="17" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="17" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="6" width="17" style="2"/>
-    <col min="7" max="7" width="22.375" style="2" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="17" style="2"/>
-    <col min="9" max="9" width="22.875" style="2" customWidth="1"/>
-    <col min="10" max="10" width="29.375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="25.875" style="2" customWidth="1"/>
+    <col min="9" max="9" width="22.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="29.42578125" style="2" customWidth="1"/>
+    <col min="11" max="11" width="25.85546875" style="2" customWidth="1"/>
     <col min="12" max="16384" width="17" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="40.5">
+    <row r="1" spans="1:11" ht="75">
       <c r="A1" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:11" s="1" customFormat="1">
+    <row r="3" spans="1:11" s="1" customFormat="1" ht="30">
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
@@ -863,7 +885,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="4" spans="1:11">
+    <row r="4" spans="1:11" ht="30">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
@@ -898,7 +920,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:11">
+    <row r="5" spans="1:11" ht="30">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
@@ -933,7 +955,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="6" spans="1:11">
+    <row r="6" spans="1:11" ht="30">
       <c r="E6" s="2" t="s">
         <v>11</v>
       </c>
@@ -995,25 +1017,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O31"/>
+  <dimension ref="A1:O37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D16" workbookViewId="0">
-      <selection activeCell="K34" sqref="K34"/>
+    <sheetView tabSelected="1" topLeftCell="D10" workbookViewId="0">
+      <selection activeCell="K42" sqref="K42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="5" max="5" width="9.625" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="7" width="14.125" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" customWidth="1"/>
+    <col min="7" max="7" width="14.140625" customWidth="1"/>
     <col min="8" max="8" width="10" customWidth="1"/>
-    <col min="9" max="9" width="14.375" customWidth="1"/>
-    <col min="10" max="10" width="38.375" customWidth="1"/>
-    <col min="11" max="11" width="30.875" customWidth="1"/>
-    <col min="12" max="12" width="35.25" customWidth="1"/>
-    <col min="13" max="13" width="14.75" customWidth="1"/>
-    <col min="14" max="14" width="13.875" customWidth="1"/>
-    <col min="15" max="15" width="43.875" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="38.42578125" customWidth="1"/>
+    <col min="11" max="11" width="88.140625" customWidth="1"/>
+    <col min="12" max="12" width="35.28515625" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" customWidth="1"/>
+    <col min="15" max="15" width="43.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -1055,7 +1077,7 @@
     </row>
     <row r="3" spans="1:15">
       <c r="B3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C3" t="s">
         <v>48</v>
@@ -1079,7 +1101,7 @@
         <v>55</v>
       </c>
       <c r="J3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -1108,7 +1130,7 @@
         <v>55</v>
       </c>
       <c r="J4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -1137,12 +1159,12 @@
         <v>55</v>
       </c>
       <c r="J5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="B6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C6" t="s">
         <v>48</v>
@@ -1166,7 +1188,7 @@
         <v>55</v>
       </c>
       <c r="J6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -1195,7 +1217,7 @@
         <v>55</v>
       </c>
       <c r="J7" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1224,7 +1246,7 @@
         <v>55</v>
       </c>
       <c r="J8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1253,92 +1275,92 @@
         <v>55</v>
       </c>
       <c r="J9" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K9" t="s">
-        <v>65</v>
+        <v>102</v>
       </c>
     </row>
     <row r="11" spans="1:15" s="4" customFormat="1">
       <c r="B11" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="F11" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="G11" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="H11" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="I11" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="H11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="I11" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>77</v>
-      </c>
       <c r="K11" s="4" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O11" s="4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="13" spans="1:15" s="3" customFormat="1">
       <c r="B13" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="E13" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="F13" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="E13" s="3" t="s">
+      <c r="G13" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F13" s="3" t="s">
+      <c r="I13" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="G13" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="I13" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="J13" s="3" t="s">
-        <v>77</v>
-      </c>
       <c r="K13" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="M13" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O13" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="14" spans="1:15" s="3" customFormat="1">
@@ -1346,7 +1368,7 @@
         <v>2</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:15" s="3" customFormat="1">
@@ -1354,7 +1376,7 @@
         <v>3</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="16" spans="1:15" s="3" customFormat="1">
@@ -1362,7 +1384,7 @@
         <v>4</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="17" spans="2:15" s="3" customFormat="1">
@@ -1370,7 +1392,7 @@
         <v>5</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="18" spans="2:15" s="3" customFormat="1">
@@ -1378,7 +1400,7 @@
         <v>6</v>
       </c>
       <c r="K18" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="2:15" s="3" customFormat="1">
@@ -1386,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="K19" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="2:15" s="3" customFormat="1">
@@ -1394,7 +1416,7 @@
         <v>8</v>
       </c>
       <c r="K20" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="21" spans="2:15" s="3" customFormat="1">
@@ -1402,7 +1424,7 @@
         <v>9</v>
       </c>
       <c r="K21" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="2:15" s="3" customFormat="1">
@@ -1410,63 +1432,63 @@
         <v>10</v>
       </c>
       <c r="J22" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="K22" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="2:15" s="5" customFormat="1">
       <c r="B25" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D25" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C25" s="5" t="s">
+      <c r="E25" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="F25" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="E25" s="5" t="s">
+      <c r="G25" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>73</v>
       </c>
-      <c r="F25" s="5" t="s">
+      <c r="I25" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>78</v>
-      </c>
-      <c r="H25" s="5" t="s">
+      <c r="J25" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="I25" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="J25" s="5" t="s">
-        <v>77</v>
-      </c>
       <c r="K25" s="5" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="L25" s="5" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="M25" s="5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="O25" s="5" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" spans="2:15" s="5" customFormat="1">
       <c r="J26" s="5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="2:15" s="5" customFormat="1"/>
     <row r="28" spans="2:15" s="5" customFormat="1"/>
     <row r="30" spans="2:15">
       <c r="B30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C30" t="s">
         <v>48</v>
@@ -1490,10 +1512,10 @@
         <v>55</v>
       </c>
       <c r="J30" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K30" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="31" spans="2:15">
@@ -1522,10 +1544,150 @@
         <v>55</v>
       </c>
       <c r="J31" t="s">
+        <v>98</v>
+      </c>
+      <c r="K31" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="B33" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1</v>
+      </c>
+      <c r="D33" t="s">
+        <v>49</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" t="s">
         <v>100</v>
       </c>
-      <c r="K31" t="s">
+      <c r="H33" t="s">
+        <v>18</v>
+      </c>
+      <c r="I33" t="s">
+        <v>26</v>
+      </c>
+      <c r="J33" t="s">
         <v>101</v>
+      </c>
+      <c r="K33" t="s">
+        <v>103</v>
+      </c>
+      <c r="L33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" t="s">
+        <v>68</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" t="s">
+        <v>105</v>
+      </c>
+      <c r="H34" t="s">
+        <v>18</v>
+      </c>
+      <c r="I34" t="s">
+        <v>26</v>
+      </c>
+      <c r="J34" t="s">
+        <v>101</v>
+      </c>
+      <c r="K34" t="s">
+        <v>107</v>
+      </c>
+      <c r="L34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="2:12">
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+      <c r="C36" t="s">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>49</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" t="s">
+        <v>106</v>
+      </c>
+      <c r="H36" t="s">
+        <v>18</v>
+      </c>
+      <c r="I36" t="s">
+        <v>26</v>
+      </c>
+      <c r="J36" t="s">
+        <v>101</v>
+      </c>
+      <c r="K36" t="s">
+        <v>109</v>
+      </c>
+      <c r="L36" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="2:12">
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+      <c r="C37" t="s">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" t="s">
+        <v>106</v>
+      </c>
+      <c r="H37" t="s">
+        <v>18</v>
+      </c>
+      <c r="I37" t="s">
+        <v>26</v>
+      </c>
+      <c r="J37" t="s">
+        <v>101</v>
+      </c>
+      <c r="K37" t="s">
+        <v>109</v>
+      </c>
+      <c r="L37" t="s">
+        <v>108</v>
       </c>
     </row>
   </sheetData>
@@ -1540,7 +1702,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>